<commit_message>
ECP-806: brings turnover rent fixed maintenance back to current and previous year; displays end date previous; makes overlapping terms visible
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -27,18 +27,6 @@
     <t>Lease External Reference</t>
   </si>
   <si>
-    <t>Start Date Previous</t>
-  </si>
-  <si>
-    <t>Value Previous</t>
-  </si>
-  <si>
-    <t>Start Date Current</t>
-  </si>
-  <si>
-    <t>Value Current</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -58,6 +46,15 @@
   </si>
   <si>
     <t>4060-0090-03</t>
+  </si>
+  <si>
+    <t>Start Date Previous Year</t>
+  </si>
+  <si>
+    <t>End Date Previous Year</t>
+  </si>
+  <si>
+    <t>Value Previous Year</t>
   </si>
 </sst>
 </file>
@@ -109,8 +106,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -119,9 +124,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,27 +464,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,71 +489,74 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="C2" s="2">
         <v>40179</v>
       </c>
-      <c r="F2">
+      <c r="D2" s="1">
+        <v>40543</v>
+      </c>
+      <c r="E2">
         <v>18000</v>
       </c>
+      <c r="F2" s="1">
+        <v>40544</v>
+      </c>
       <c r="G2" s="1">
-        <v>40544</v>
+        <v>40908</v>
       </c>
       <c r="H2">
         <v>21000</v>
       </c>
-      <c r="I2" s="1">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D3" s="1">
+        <v>40543</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>40544</v>
+      </c>
+      <c r="G3" s="1">
         <v>40908</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1">
-        <v>40374</v>
-      </c>
-      <c r="F3">
-        <v>2000</v>
-      </c>
-      <c r="G3" s="2">
-        <v>40544</v>
       </c>
       <c r="H3">
         <v>2100</v>
-      </c>
-      <c r="I3" s="1">
-        <v>40908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECP-806: now import handles overlapping terms for current year; also no longer creates terms for previous years - only updates when found
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Value Previous Year</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -119,10 +122,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -464,11 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -479,9 +483,10 @@
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,8 +511,11 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -532,8 +540,11 @@
       <c r="H2">
         <v>21000</v>
       </c>
+      <c r="I2" s="3">
+        <v>2011</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -557,6 +568,9 @@
       </c>
       <c r="H3">
         <v>2100</v>
+      </c>
+      <c r="I3">
+        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECP-1107: sets up revised import and tests
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2827935-C84D-6248-8585-1D1B60252639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33360" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lease terms" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -58,12 +64,15 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -143,6 +152,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -467,26 +484,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,10 +531,13 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -540,11 +562,14 @@
       <c r="H2">
         <v>21000</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3">
         <v>2011</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -570,6 +595,9 @@
         <v>2100</v>
       </c>
       <c r="I3">
+        <v>3.6</v>
+      </c>
+      <c r="J3">
         <v>2011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ECP-1107: importing splits term when comprises more than a year & turnover rent rule copied from previous term when left empty
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maredupreez/ECP/estatio-ecp-mare/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2827935-C84D-6248-8585-1D1B60252639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33360" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33360" windowHeight="18180"/>
   </bookViews>
   <sheets>
     <sheet name="lease terms" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -72,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -484,12 +486,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -601,13 +603,69 @@
         <v>2011</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>40544</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40908</v>
+      </c>
+      <c r="E4">
+        <v>2100</v>
+      </c>
+      <c r="F4" s="2">
+        <v>40909</v>
+      </c>
+      <c r="G4" s="2">
+        <v>41639</v>
+      </c>
+      <c r="H4">
+        <v>2200</v>
+      </c>
+      <c r="I4">
+        <v>3.6</v>
+      </c>
+      <c r="J4">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>41275</v>
+      </c>
+      <c r="D5" s="2">
+        <v>41639</v>
+      </c>
+      <c r="E5">
+        <v>2300</v>
+      </c>
+      <c r="F5" s="2">
+        <v>41640</v>
+      </c>
+      <c r="G5" s="2">
+        <v>42004</v>
+      </c>
+      <c r="H5">
+        <v>2300</v>
+      </c>
+      <c r="J5">
+        <v>2014</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ECP-1107: extended integ test for importing term with missing percentage
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -487,11 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,34 +573,24 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D3" s="1">
-        <v>40543</v>
-      </c>
-      <c r="E3">
-        <v>2000</v>
-      </c>
-      <c r="F3" s="2">
-        <v>40544</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1">
+        <v>41275</v>
       </c>
       <c r="G3" s="1">
-        <v>40908</v>
+        <v>41639</v>
       </c>
       <c r="H3">
-        <v>2100</v>
-      </c>
-      <c r="I3">
-        <v>3.6</v>
-      </c>
-      <c r="J3">
-        <v>2011</v>
+        <v>23000</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2013</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -610,29 +600,29 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40543</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="F4" s="2">
         <v>40544</v>
       </c>
-      <c r="D4" s="1">
+      <c r="G4" s="1">
         <v>40908</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>2100</v>
-      </c>
-      <c r="F4" s="2">
-        <v>40909</v>
-      </c>
-      <c r="G4" s="2">
-        <v>41639</v>
-      </c>
-      <c r="H4">
-        <v>2200</v>
       </c>
       <c r="I4">
         <v>3.6</v>
       </c>
       <c r="J4">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -643,26 +633,65 @@
         <v>8</v>
       </c>
       <c r="C5" s="2">
+        <v>40544</v>
+      </c>
+      <c r="D5" s="1">
+        <v>40908</v>
+      </c>
+      <c r="E5">
+        <v>2100</v>
+      </c>
+      <c r="F5" s="2">
+        <v>40909</v>
+      </c>
+      <c r="G5" s="2">
+        <v>41639</v>
+      </c>
+      <c r="H5">
+        <v>2200</v>
+      </c>
+      <c r="I5">
+        <v>3.6</v>
+      </c>
+      <c r="J5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
         <v>41275</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>41639</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>2300</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>41640</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G6" s="2">
         <v>42004</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>2300</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <v>2014</v>
       </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="J7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>